<commit_message>
needs to ve fixed
</commit_message>
<xml_diff>
--- a/basic_page.xlsx
+++ b/basic_page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/purva/Desktop/SUNY Geneseo Playwright/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C9B7AB-A217-3F40-A8DA-03686DFE42BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462CB370-EA17-464C-810F-9DD924C5DBD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,35 +22,42 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>finalUrl</t>
-  </si>
-  <si>
-    <t>http://drupal-geneseo-backup.ddev.site/basic_page/boiling-flasks-round-bottom/</t>
-  </si>
-  <si>
-    <t>http://drupal-geneseo-backup.ddev.site/academics</t>
-  </si>
-  <si>
-    <t>http://drupal-geneseo-backup.ddev.site/basic_page/mofs-part-3/</t>
-  </si>
-  <si>
-    <t>http://drupal-geneseo-backup.ddev.site/basic_page/journals-and-reflections/</t>
-  </si>
-  <si>
-    <t>http://drupal-geneseo-backup.ddev.site/basic_page/conh35clcl2-prep/</t>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>/basic_page/applied-biosystems-model-7000-real-time-thermalcycler/</t>
+  </si>
+  <si>
+    <t>/basic_page/105-description/</t>
+  </si>
+  <si>
+    <t>/basic_page/119-description/</t>
+  </si>
+  <si>
+    <t>/basic_page/209-description/</t>
+  </si>
+  <si>
+    <t>/basic_page/216-description/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -61,15 +68,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,14 +90,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -391,34 +416,34 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="89.83203125" customWidth="1"/>
+    <col min="1" max="1" width="80" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -432,12 +457,10 @@
         <v>5</v>
       </c>
     </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://dev-infostride-geneseo.pantheonsite.io/basic_page/boiling-flasks-round-bottom/" xr:uid="{4C5C5195-89FA-5E48-8B12-A05BD4B66193}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://dev-infostride-geneseo.pantheonsite.io/academics" xr:uid="{B231DE5C-3933-C24A-9AAC-3CF15448C454}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://dev-infostride-geneseo.pantheonsite.io/basic_page/mofs-part-3/" xr:uid="{211FAB93-E79E-EB4F-8E0C-4FA5A0B9DBCD}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed for one browser
</commit_message>
<xml_diff>
--- a/basic_page.xlsx
+++ b/basic_page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/purva/Desktop/SUNY Geneseo Playwright/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462CB370-EA17-464C-810F-9DD924C5DBD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F825369C-0DC7-7645-999E-238600495C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,24 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Path</t>
   </si>
   <si>
     <t>/basic_page/applied-biosystems-model-7000-real-time-thermalcycler/</t>
-  </si>
-  <si>
-    <t>/basic_page/105-description/</t>
-  </si>
-  <si>
-    <t>/basic_page/119-description/</t>
-  </si>
-  <si>
-    <t>/basic_page/209-description/</t>
-  </si>
-  <si>
-    <t>/basic_page/216-description/</t>
   </si>
 </sst>
 </file>
@@ -419,7 +407,7 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -437,26 +425,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
     </row>

</xml_diff>

<commit_message>
fixed cache for slugs, fixing for validatechildlinks
</commit_message>
<xml_diff>
--- a/basic_page.xlsx
+++ b/basic_page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/purva/Desktop/SUNY Geneseo Playwright/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639FFE65-1F67-8041-BF00-D504216E617E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56159C57-F183-5243-AF4C-9EA5FAE4D30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="449">
   <si>
     <t>urso</t>
   </si>
@@ -1368,298 +1368,32 @@
     <t>rivera</t>
   </si>
   <si>
-    <t>Path</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/astrophysics</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/anthropology</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/cognitive-science</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/applied-physics</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/astronomy</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/applied-mathematics</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/art-history</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/biochemistry</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/accounting</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/biology</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/black-and-africana-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/business-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/cultural-studies-41</t>
-  </si>
-  <si>
     <t>/academic-program-finder/mba-41</t>
   </si>
   <si>
-    <t>/academic-program-finder/biophysics</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/communication</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/dance</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/chemistry</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/conflict-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/economics</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/entrepreneurship</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/data-analytics</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/engineering-32</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/finance</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/european-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/film-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/ethics-and-values-society</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/geography</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/geochemistry</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/history</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/human-resources-management</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/german</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/jazz-and-american-music-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/human-development</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/international-relations</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/legal-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/latin-american-and-caribbean-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/linguistics</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/multidisciplinary-creative-practice</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/music</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/medieval-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/museum-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/music-composition</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/geophysics</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/geological-sciences</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/music-conducting</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/physics</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/neuroscience</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/political-science</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/piano-pedagogy</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/psychology</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/pre-professional-studies-music-teaching-k-12</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/queer-and-sexuality-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/public-administration</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/sociology</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/religious-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/spanish</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/sociomedical-sciences</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/musical-theatre</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/sustainable-systems-41</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/music-business-recording-and-production</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/sustainability-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/theatre</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/urban-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/accounting-masters</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/philosophy-politics-and-economics</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/individualized-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/law-33</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/history-masters</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/marketing</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/chiropractic-medicine-33-and-43</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/dentistry-44</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/pharmacy-34</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/osteopathic-44</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/podiatry-44</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/optometry-34</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/asian-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/physical-therapy-33</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/american-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/english</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/comparative-literature</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/mathematics</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/native-american-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/french</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/philosophy</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/womens-and-gender-studies</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/adolescence-education</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/business-administration</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/early-childhood-and-childhood-education</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/reading-and-literacy</t>
-  </si>
-  <si>
-    <t>/academic-program-finder/teaching-students-disabilities-childhood-education</t>
+    <t>/hr/performance-management%C2%A0tools-resources</t>
+  </si>
+  <si>
+    <t>CPT</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>VD</t>
+  </si>
+  <si>
+    <t>Slug</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1671,27 +1405,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4BACC6"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1718,22 +1438,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2037,10 +1751,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B482"/>
+  <dimension ref="A1:B470"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2049,1732 +1763,1432 @@
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>443</v>
-      </c>
-      <c r="B1" s="2"/>
+        <v>445</v>
+      </c>
+      <c r="B1" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B2" t="s">
         <v>444</v>
       </c>
-      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>445</v>
-      </c>
-      <c r="B3" s="3"/>
+        <v>447</v>
+      </c>
+      <c r="B3" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>446</v>
-      </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>447</v>
-      </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>448</v>
-      </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>449</v>
-      </c>
-      <c r="B7" s="3"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>450</v>
-      </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>451</v>
-      </c>
-      <c r="B9" s="3"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>453</v>
-      </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>454</v>
-      </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>455</v>
-      </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>456</v>
-      </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>457</v>
-      </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>458</v>
-      </c>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>459</v>
-      </c>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>460</v>
-      </c>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>461</v>
-      </c>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>462</v>
-      </c>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>463</v>
-      </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>464</v>
-      </c>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>465</v>
-      </c>
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>466</v>
-      </c>
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>467</v>
-      </c>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>468</v>
-      </c>
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>469</v>
-      </c>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>470</v>
-      </c>
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>471</v>
-      </c>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>472</v>
-      </c>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>473</v>
-      </c>
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>474</v>
-      </c>
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>475</v>
-      </c>
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>476</v>
-      </c>
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>477</v>
-      </c>
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>478</v>
-      </c>
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>479</v>
-      </c>
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>480</v>
-      </c>
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>481</v>
-      </c>
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>482</v>
-      </c>
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>483</v>
-      </c>
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>484</v>
-      </c>
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>485</v>
-      </c>
-      <c r="B43" s="3"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>486</v>
-      </c>
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>487</v>
-      </c>
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>488</v>
-      </c>
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>489</v>
-      </c>
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>490</v>
-      </c>
-      <c r="B48" s="3"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>491</v>
-      </c>
-      <c r="B49" s="3"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>492</v>
-      </c>
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>493</v>
-      </c>
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>494</v>
-      </c>
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>495</v>
-      </c>
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>496</v>
-      </c>
-      <c r="B54" s="3"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>497</v>
-      </c>
-      <c r="B55" s="3"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>498</v>
-      </c>
-      <c r="B56" s="3"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>499</v>
-      </c>
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>500</v>
-      </c>
-      <c r="B58" s="3"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>501</v>
-      </c>
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>502</v>
-      </c>
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>503</v>
-      </c>
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>504</v>
-      </c>
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>505</v>
-      </c>
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>506</v>
-      </c>
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>507</v>
-      </c>
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>508</v>
-      </c>
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>509</v>
-      </c>
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>510</v>
-      </c>
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>511</v>
-      </c>
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>512</v>
-      </c>
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>513</v>
-      </c>
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>514</v>
-      </c>
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>515</v>
-      </c>
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>516</v>
-      </c>
-      <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>517</v>
-      </c>
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>518</v>
-      </c>
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>519</v>
-      </c>
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>520</v>
-      </c>
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>521</v>
-      </c>
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>522</v>
-      </c>
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>523</v>
-      </c>
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>524</v>
-      </c>
-      <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>525</v>
-      </c>
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>526</v>
-      </c>
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>527</v>
-      </c>
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>528</v>
-      </c>
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>529</v>
-      </c>
-      <c r="B87" s="3"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>530</v>
-      </c>
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>531</v>
-      </c>
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>532</v>
-      </c>
-      <c r="B90" s="3"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>533</v>
-      </c>
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>534</v>
-      </c>
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B94" s="3"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B95" s="3"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B96" s="3"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B96" s="1"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B97" s="3"/>
+      <c r="B97" s="1"/>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B98" s="3"/>
+      <c r="B98" s="1"/>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B99" s="3"/>
+      <c r="B99" s="1"/>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B100" s="3"/>
+      <c r="B100" s="1"/>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B101" s="3"/>
+      <c r="B101" s="1"/>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B102" s="3"/>
+      <c r="B102" s="1"/>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B103" s="3"/>
+      <c r="B103" s="1"/>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B104" s="3"/>
+      <c r="B104" s="1"/>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B105" s="3"/>
+      <c r="B105" s="1"/>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B106" s="3"/>
+      <c r="B106" s="1"/>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B107" s="3"/>
+      <c r="B107" s="1"/>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B108" s="3"/>
+      <c r="B108" s="1"/>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B109" s="3"/>
+      <c r="B109" s="1"/>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B110" s="3"/>
+      <c r="B110" s="1"/>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B111" s="3"/>
+      <c r="B111" s="1"/>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B112" s="3"/>
+      <c r="B112" s="1"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B113" s="3"/>
+      <c r="B113" s="1"/>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B114" s="3"/>
+      <c r="B114" s="1"/>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B115" s="3"/>
+      <c r="B115" s="1"/>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B116" s="3"/>
+      <c r="B116" s="1"/>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B117" s="3"/>
+      <c r="B117" s="1"/>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B118" s="3"/>
+      <c r="B118" s="1"/>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B119" s="3"/>
+      <c r="B119" s="1"/>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B120" s="3"/>
+      <c r="B120" s="1"/>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B121" s="3"/>
+      <c r="B121" s="1"/>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B122" s="3"/>
+      <c r="B122" s="1"/>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B123" s="3"/>
+      <c r="B123" s="1"/>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B124" s="3"/>
+      <c r="B124" s="1"/>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B125" s="3"/>
+      <c r="B125" s="1"/>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B126" s="3"/>
+      <c r="B126" s="1"/>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B127" s="3"/>
+      <c r="B127" s="1"/>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B128" s="3"/>
+      <c r="B128" s="1"/>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B129" s="3"/>
+      <c r="B129" s="1"/>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B130" s="3"/>
+      <c r="B130" s="1"/>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B131" s="3"/>
+      <c r="B131" s="1"/>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B132" s="3"/>
+      <c r="B132" s="1"/>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B133" s="3"/>
+      <c r="B133" s="1"/>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B134" s="3"/>
+      <c r="B134" s="1"/>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B135" s="3"/>
+      <c r="B135" s="1"/>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B136" s="3"/>
+      <c r="B136" s="1"/>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B137" s="3"/>
+      <c r="B137" s="1"/>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B138" s="3"/>
+      <c r="B138" s="1"/>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B139" s="3"/>
+      <c r="B139" s="1"/>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B140" s="3"/>
+      <c r="B140" s="1"/>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B141" s="3"/>
+      <c r="B141" s="1"/>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B142" s="3"/>
+      <c r="B142" s="1"/>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B143" s="3"/>
+      <c r="B143" s="1"/>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B144" s="3"/>
+      <c r="B144" s="1"/>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B145" s="3"/>
+      <c r="B145" s="1"/>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B146" s="3"/>
+      <c r="B146" s="1"/>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B147" s="3"/>
+      <c r="B147" s="1"/>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B148" s="3"/>
+      <c r="B148" s="1"/>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B149" s="3"/>
+      <c r="B149" s="1"/>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B150" s="3"/>
+      <c r="B150" s="1"/>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B151" s="3"/>
+      <c r="B151" s="1"/>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B152" s="3"/>
+      <c r="B152" s="1"/>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B153" s="3"/>
+      <c r="B153" s="1"/>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B154" s="3"/>
+      <c r="B154" s="1"/>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B155" s="3"/>
+      <c r="B155" s="1"/>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B156" s="3"/>
+      <c r="B156" s="1"/>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B157" s="3"/>
+      <c r="B157" s="1"/>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B158" s="3"/>
+      <c r="B158" s="1"/>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B159" s="3"/>
+      <c r="B159" s="1"/>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B160" s="3"/>
+      <c r="B160" s="1"/>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B161" s="3"/>
+      <c r="B161" s="1"/>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B162" s="3"/>
+      <c r="B162" s="1"/>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B163" s="3"/>
+      <c r="B163" s="1"/>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B164" s="3"/>
+      <c r="B164" s="1"/>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B165" s="3"/>
+      <c r="B165" s="1"/>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B166" s="3"/>
+      <c r="B166" s="1"/>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B167" s="3"/>
+      <c r="B167" s="1"/>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B168" s="3"/>
+      <c r="B168" s="1"/>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B169" s="3"/>
+      <c r="B169" s="1"/>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B170" s="3"/>
+      <c r="B170" s="1"/>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B171" s="3"/>
+      <c r="B171" s="1"/>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B172" s="3"/>
+      <c r="B172" s="1"/>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B173" s="3"/>
+      <c r="B173" s="1"/>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B174" s="3"/>
+      <c r="B174" s="1"/>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B175" s="3"/>
+      <c r="B175" s="1"/>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B176" s="3"/>
+      <c r="B176" s="1"/>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B177" s="3"/>
+      <c r="B177" s="1"/>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B178" s="3"/>
+      <c r="B178" s="1"/>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B179" s="3"/>
+      <c r="B179" s="1"/>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B180" s="3"/>
+      <c r="B180" s="1"/>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B181" s="3"/>
+      <c r="B181" s="1"/>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B182" s="3"/>
+      <c r="B182" s="1"/>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B183" s="3"/>
+      <c r="B183" s="1"/>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B184" s="3"/>
+      <c r="B184" s="1"/>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B185" s="3"/>
+      <c r="B185" s="1"/>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B186" s="3"/>
+      <c r="B186" s="1"/>
     </row>
     <row r="187" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B187" s="3"/>
+      <c r="B187" s="1"/>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B188" s="3"/>
+      <c r="B188" s="1"/>
     </row>
     <row r="189" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B189" s="3"/>
+      <c r="B189" s="1"/>
     </row>
     <row r="190" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B190" s="3"/>
+      <c r="B190" s="1"/>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B191" s="3"/>
+      <c r="B191" s="1"/>
     </row>
     <row r="192" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B192" s="3"/>
+      <c r="B192" s="1"/>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B193" s="3"/>
+      <c r="B193" s="1"/>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B194" s="3"/>
+      <c r="B194" s="1"/>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B195" s="3"/>
+      <c r="B195" s="1"/>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B196" s="3"/>
+      <c r="B196" s="1"/>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B197" s="3"/>
+      <c r="B197" s="1"/>
     </row>
     <row r="198" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B198" s="3"/>
+      <c r="B198" s="1"/>
     </row>
     <row r="199" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B199" s="3"/>
+      <c r="B199" s="1"/>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B200" s="3"/>
+      <c r="B200" s="1"/>
     </row>
     <row r="201" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B201" s="3"/>
+      <c r="B201" s="1"/>
     </row>
     <row r="202" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B202" s="3"/>
+      <c r="B202" s="1"/>
     </row>
     <row r="203" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B203" s="3"/>
+      <c r="B203" s="1"/>
     </row>
     <row r="204" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B204" s="3"/>
+      <c r="B204" s="1"/>
     </row>
     <row r="205" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B205" s="3"/>
+      <c r="B205" s="1"/>
     </row>
     <row r="206" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B206" s="3"/>
+      <c r="B206" s="1"/>
     </row>
     <row r="207" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B207" s="3"/>
+      <c r="B207" s="1"/>
     </row>
     <row r="208" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B208" s="3"/>
+      <c r="B208" s="1"/>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B209" s="3"/>
+      <c r="B209" s="1"/>
     </row>
     <row r="210" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B210" s="3"/>
+      <c r="B210" s="1"/>
     </row>
     <row r="211" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B211" s="3"/>
+      <c r="B211" s="1"/>
     </row>
     <row r="212" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B212" s="3"/>
+      <c r="B212" s="1"/>
     </row>
     <row r="213" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B213" s="3"/>
+      <c r="B213" s="1"/>
     </row>
     <row r="214" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B214" s="3"/>
+      <c r="B214" s="1"/>
     </row>
     <row r="215" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B215" s="3"/>
+      <c r="B215" s="1"/>
     </row>
     <row r="216" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B216" s="3"/>
+      <c r="B216" s="1"/>
     </row>
     <row r="217" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B217" s="3"/>
+      <c r="B217" s="1"/>
     </row>
     <row r="218" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B218" s="3"/>
+      <c r="B218" s="1"/>
     </row>
     <row r="219" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B219" s="3"/>
+      <c r="B219" s="1"/>
     </row>
     <row r="220" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B220" s="3"/>
+      <c r="B220" s="1"/>
     </row>
     <row r="221" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B221" s="3"/>
+      <c r="B221" s="1"/>
     </row>
     <row r="222" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B222" s="3"/>
+      <c r="B222" s="1"/>
     </row>
     <row r="223" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B223" s="3"/>
+      <c r="B223" s="1"/>
     </row>
     <row r="224" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B224" s="3"/>
+      <c r="B224" s="1"/>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B225" s="3"/>
+      <c r="B225" s="1"/>
     </row>
     <row r="226" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B226" s="3"/>
+      <c r="B226" s="1"/>
     </row>
     <row r="227" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B227" s="3"/>
+      <c r="B227" s="1"/>
     </row>
     <row r="228" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B228" s="3"/>
+      <c r="B228" s="1"/>
     </row>
     <row r="229" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B229" s="3"/>
+      <c r="B229" s="1"/>
     </row>
     <row r="230" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B230" s="3"/>
+      <c r="B230" s="1"/>
     </row>
     <row r="231" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B231" s="3"/>
+      <c r="B231" s="1"/>
     </row>
     <row r="232" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B232" s="3"/>
+      <c r="B232" s="1"/>
     </row>
     <row r="233" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B233" s="3"/>
+      <c r="B233" s="1"/>
     </row>
     <row r="234" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B234" s="3"/>
+      <c r="B234" s="1"/>
     </row>
     <row r="235" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B235" s="3"/>
+      <c r="B235" s="1"/>
     </row>
     <row r="236" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B236" s="3"/>
+      <c r="B236" s="1"/>
     </row>
     <row r="237" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B237" s="3"/>
+      <c r="B237" s="1"/>
     </row>
     <row r="238" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B238" s="3"/>
+      <c r="B238" s="1"/>
     </row>
     <row r="239" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B239" s="3"/>
+      <c r="B239" s="1"/>
     </row>
     <row r="240" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B240" s="3"/>
+      <c r="B240" s="1"/>
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B241" s="3"/>
+      <c r="B241" s="1"/>
     </row>
     <row r="242" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B242" s="3"/>
+      <c r="B242" s="1"/>
     </row>
     <row r="243" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B243" s="3"/>
+      <c r="B243" s="1"/>
     </row>
     <row r="244" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B244" s="3"/>
+      <c r="B244" s="1"/>
     </row>
     <row r="245" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B245" s="3"/>
+      <c r="B245" s="1"/>
     </row>
     <row r="246" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B246" s="3"/>
+      <c r="B246" s="1"/>
     </row>
     <row r="247" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B247" s="3"/>
+      <c r="B247" s="1"/>
     </row>
     <row r="248" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B248" s="3"/>
+      <c r="B248" s="1"/>
     </row>
     <row r="249" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B249" s="3"/>
+      <c r="B249" s="1"/>
     </row>
     <row r="250" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B250" s="3"/>
+      <c r="B250" s="1"/>
     </row>
     <row r="251" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B251" s="3"/>
+      <c r="B251" s="1"/>
     </row>
     <row r="252" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B252" s="3"/>
+      <c r="B252" s="1"/>
     </row>
     <row r="253" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B253" s="3"/>
+      <c r="B253" s="1"/>
     </row>
     <row r="254" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B254" s="3"/>
+      <c r="B254" s="1"/>
     </row>
     <row r="255" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B255" s="3"/>
+      <c r="B255" s="1"/>
     </row>
     <row r="256" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B256" s="3"/>
+      <c r="B256" s="1"/>
     </row>
     <row r="257" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B257" s="3"/>
+      <c r="B257" s="1"/>
     </row>
     <row r="258" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B258" s="3"/>
+      <c r="B258" s="1"/>
     </row>
     <row r="259" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B259" s="3"/>
+      <c r="B259" s="1"/>
     </row>
     <row r="260" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B260" s="3"/>
+      <c r="B260" s="1"/>
     </row>
     <row r="261" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B261" s="3"/>
+      <c r="B261" s="1"/>
     </row>
     <row r="262" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B262" s="3"/>
+      <c r="B262" s="1"/>
     </row>
     <row r="263" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B263" s="3"/>
+      <c r="B263" s="1"/>
     </row>
     <row r="264" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B264" s="3"/>
+      <c r="B264" s="1"/>
     </row>
     <row r="265" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B265" s="3"/>
+      <c r="B265" s="1"/>
     </row>
     <row r="266" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B266" s="3"/>
+      <c r="B266" s="1"/>
     </row>
     <row r="267" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B267" s="3"/>
+      <c r="B267" s="1"/>
     </row>
     <row r="268" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B268" s="3"/>
+      <c r="B268" s="1"/>
     </row>
     <row r="269" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B269" s="3"/>
+      <c r="B269" s="1"/>
     </row>
     <row r="270" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B270" s="3"/>
+      <c r="B270" s="1"/>
     </row>
     <row r="271" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B271" s="3"/>
+      <c r="B271" s="1"/>
     </row>
     <row r="272" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B272" s="3"/>
+      <c r="B272" s="1"/>
     </row>
     <row r="273" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B273" s="3"/>
+      <c r="B273" s="1"/>
     </row>
     <row r="274" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B274" s="3"/>
+      <c r="B274" s="1"/>
     </row>
     <row r="275" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B275" s="3"/>
+      <c r="B275" s="1"/>
     </row>
     <row r="276" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B276" s="3"/>
+      <c r="B276" s="1"/>
     </row>
     <row r="277" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B277" s="3"/>
+      <c r="B277" s="1"/>
     </row>
     <row r="278" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B278" s="3"/>
+      <c r="B278" s="1"/>
     </row>
     <row r="279" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B279" s="3"/>
+      <c r="B279" s="1"/>
     </row>
     <row r="280" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B280" s="3"/>
+      <c r="B280" s="1"/>
     </row>
     <row r="281" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B281" s="3"/>
+      <c r="B281" s="1"/>
     </row>
     <row r="282" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B282" s="3"/>
+      <c r="B282" s="1"/>
     </row>
     <row r="283" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B283" s="3"/>
+      <c r="B283" s="1"/>
     </row>
     <row r="284" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B284" s="3"/>
+      <c r="B284" s="1"/>
     </row>
     <row r="285" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B285" s="3"/>
+      <c r="B285" s="1"/>
     </row>
     <row r="286" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B286" s="3"/>
+      <c r="B286" s="1"/>
     </row>
     <row r="287" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B287" s="3"/>
+      <c r="B287" s="1"/>
     </row>
     <row r="288" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B288" s="3"/>
+      <c r="B288" s="1"/>
     </row>
     <row r="289" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B289" s="3"/>
+      <c r="B289" s="1"/>
     </row>
     <row r="290" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B290" s="3"/>
+      <c r="B290" s="1"/>
     </row>
     <row r="291" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B291" s="3"/>
+      <c r="B291" s="1"/>
     </row>
     <row r="292" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B292" s="3"/>
+      <c r="B292" s="1"/>
     </row>
     <row r="293" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B293" s="3"/>
+      <c r="B293" s="1"/>
     </row>
     <row r="294" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B294" s="3"/>
+      <c r="B294" s="1"/>
     </row>
     <row r="295" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B295" s="3"/>
+      <c r="B295" s="1"/>
     </row>
     <row r="296" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B296" s="3"/>
+      <c r="B296" s="1"/>
     </row>
     <row r="297" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B297" s="3"/>
+      <c r="B297" s="1"/>
     </row>
     <row r="298" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B298" s="3"/>
+      <c r="B298" s="1"/>
     </row>
     <row r="299" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B299" s="3"/>
+      <c r="B299" s="1"/>
     </row>
     <row r="300" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B300" s="3"/>
+      <c r="B300" s="1"/>
     </row>
     <row r="301" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B301" s="3"/>
+      <c r="B301" s="1"/>
     </row>
     <row r="302" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B302" s="3"/>
+      <c r="B302" s="1"/>
     </row>
     <row r="303" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B303" s="3"/>
+      <c r="B303" s="1"/>
     </row>
     <row r="304" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B304" s="3"/>
+      <c r="B304" s="1"/>
     </row>
     <row r="305" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B305" s="3"/>
+      <c r="B305" s="1"/>
     </row>
     <row r="306" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B306" s="3"/>
+      <c r="B306" s="1"/>
     </row>
     <row r="307" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B307" s="3"/>
+      <c r="B307" s="1"/>
     </row>
     <row r="308" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B308" s="3"/>
+      <c r="B308" s="1"/>
     </row>
     <row r="309" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B309" s="3"/>
+      <c r="B309" s="1"/>
     </row>
     <row r="310" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B310" s="3"/>
+      <c r="B310" s="1"/>
     </row>
     <row r="311" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B311" s="3"/>
+      <c r="B311" s="1"/>
     </row>
     <row r="312" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B312" s="3"/>
+      <c r="B312" s="1"/>
     </row>
     <row r="313" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B313" s="3"/>
+      <c r="B313" s="1"/>
     </row>
     <row r="314" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B314" s="3"/>
+      <c r="B314" s="1"/>
     </row>
     <row r="315" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B315" s="3"/>
+      <c r="B315" s="1"/>
     </row>
     <row r="316" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B316" s="3"/>
+      <c r="B316" s="1"/>
     </row>
     <row r="317" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B317" s="3"/>
+      <c r="B317" s="1"/>
     </row>
     <row r="318" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B318" s="3"/>
+      <c r="B318" s="1"/>
     </row>
     <row r="319" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B319" s="3"/>
+      <c r="B319" s="1"/>
     </row>
     <row r="320" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B320" s="3"/>
+      <c r="B320" s="1"/>
     </row>
     <row r="321" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B321" s="3"/>
+      <c r="B321" s="1"/>
     </row>
     <row r="322" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B322" s="3"/>
+      <c r="B322" s="1"/>
     </row>
     <row r="323" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B323" s="3"/>
+      <c r="B323" s="1"/>
     </row>
     <row r="324" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B324" s="3"/>
+      <c r="B324" s="1"/>
     </row>
     <row r="325" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B325" s="3"/>
+      <c r="B325" s="1"/>
     </row>
     <row r="326" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B326" s="3"/>
+      <c r="B326" s="1"/>
     </row>
     <row r="327" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B327" s="3"/>
+      <c r="B327" s="1"/>
     </row>
     <row r="328" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B328" s="3"/>
+      <c r="B328" s="1"/>
     </row>
     <row r="329" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B329" s="3"/>
+      <c r="B329" s="1"/>
     </row>
     <row r="330" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B330" s="3"/>
+      <c r="B330" s="1"/>
     </row>
     <row r="331" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B331" s="3"/>
+      <c r="B331" s="1"/>
     </row>
     <row r="332" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B332" s="3"/>
+      <c r="B332" s="1"/>
     </row>
     <row r="333" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B333" s="3"/>
+      <c r="B333" s="1"/>
     </row>
     <row r="334" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B334" s="3"/>
+      <c r="B334" s="1"/>
     </row>
     <row r="335" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B335" s="3"/>
+      <c r="B335" s="1"/>
     </row>
     <row r="336" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B336" s="3"/>
+      <c r="B336" s="1"/>
     </row>
     <row r="337" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B337" s="3"/>
+      <c r="B337" s="1"/>
     </row>
     <row r="338" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B338" s="3"/>
+      <c r="B338" s="1"/>
     </row>
     <row r="339" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B339" s="3"/>
+      <c r="B339" s="1"/>
     </row>
     <row r="340" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B340" s="3"/>
+      <c r="B340" s="1"/>
     </row>
     <row r="341" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B341" s="3"/>
+      <c r="B341" s="1"/>
     </row>
     <row r="342" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B342" s="3"/>
+      <c r="B342" s="1"/>
     </row>
     <row r="343" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B343" s="3"/>
+      <c r="B343" s="1"/>
     </row>
     <row r="344" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B344" s="3"/>
+      <c r="B344" s="1"/>
     </row>
     <row r="345" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B345" s="3"/>
+      <c r="B345" s="1"/>
     </row>
     <row r="346" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B346" s="3"/>
+      <c r="B346" s="1"/>
     </row>
     <row r="347" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B347" s="3"/>
+      <c r="B347" s="1"/>
     </row>
     <row r="348" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B348" s="3"/>
+      <c r="B348" s="1"/>
     </row>
     <row r="349" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B349" s="3"/>
+      <c r="B349" s="1"/>
     </row>
     <row r="350" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B350" s="3"/>
+      <c r="B350" s="1"/>
     </row>
     <row r="351" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B351" s="3"/>
+      <c r="B351" s="1"/>
     </row>
     <row r="352" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B352" s="3"/>
+      <c r="B352" s="1"/>
     </row>
     <row r="353" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B353" s="3"/>
+      <c r="B353" s="1"/>
     </row>
     <row r="354" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B354" s="3"/>
+      <c r="B354" s="1"/>
     </row>
     <row r="355" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B355" s="3"/>
+      <c r="B355" s="1"/>
     </row>
     <row r="356" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B356" s="3"/>
+      <c r="B356" s="1"/>
     </row>
     <row r="357" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B357" s="3"/>
+      <c r="B357" s="1"/>
     </row>
     <row r="358" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B358" s="3"/>
+      <c r="B358" s="1"/>
     </row>
     <row r="359" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B359" s="3"/>
+      <c r="B359" s="1"/>
     </row>
     <row r="360" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B360" s="3"/>
+      <c r="B360" s="1"/>
     </row>
     <row r="361" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B361" s="3"/>
+      <c r="B361" s="1"/>
     </row>
     <row r="362" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B362" s="3"/>
+      <c r="B362" s="1"/>
     </row>
     <row r="363" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B363" s="3"/>
+      <c r="B363" s="1"/>
     </row>
     <row r="364" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B364" s="3"/>
+      <c r="B364" s="1"/>
     </row>
     <row r="365" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B365" s="3"/>
+      <c r="B365" s="1"/>
     </row>
     <row r="366" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B366" s="3"/>
+      <c r="B366" s="1"/>
     </row>
     <row r="367" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B367" s="3"/>
+      <c r="B367" s="1"/>
     </row>
     <row r="368" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B368" s="3"/>
+      <c r="B368" s="1"/>
     </row>
     <row r="369" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B369" s="3"/>
+      <c r="B369" s="1"/>
     </row>
     <row r="370" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B370" s="3"/>
+      <c r="B370" s="1"/>
     </row>
     <row r="371" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B371" s="3"/>
+      <c r="B371" s="1"/>
     </row>
     <row r="372" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B372" s="3"/>
+      <c r="B372" s="1"/>
     </row>
     <row r="373" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B373" s="3"/>
+      <c r="B373" s="1"/>
     </row>
     <row r="374" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B374" s="3"/>
+      <c r="B374" s="1"/>
     </row>
     <row r="375" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B375" s="3"/>
+      <c r="B375" s="1"/>
     </row>
     <row r="376" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B376" s="3"/>
+      <c r="B376" s="1"/>
     </row>
     <row r="377" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B377" s="3"/>
+      <c r="B377" s="1"/>
     </row>
     <row r="378" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B378" s="3"/>
+      <c r="B378" s="1"/>
     </row>
     <row r="379" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B379" s="3"/>
+      <c r="B379" s="1"/>
     </row>
     <row r="380" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B380" s="3"/>
+      <c r="B380" s="1"/>
     </row>
     <row r="381" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B381" s="3"/>
+      <c r="B381" s="1"/>
     </row>
     <row r="382" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B382" s="3"/>
+      <c r="B382" s="1"/>
     </row>
     <row r="383" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B383" s="3"/>
+      <c r="B383" s="1"/>
     </row>
     <row r="384" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B384" s="3"/>
+      <c r="B384" s="1"/>
     </row>
     <row r="385" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B385" s="3"/>
+      <c r="B385" s="1"/>
     </row>
     <row r="386" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B386" s="3"/>
+      <c r="B386" s="1"/>
     </row>
     <row r="387" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B387" s="3"/>
+      <c r="B387" s="1"/>
     </row>
     <row r="388" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B388" s="3"/>
+      <c r="B388" s="1"/>
     </row>
     <row r="389" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B389" s="3"/>
+      <c r="B389" s="1"/>
     </row>
     <row r="390" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B390" s="3"/>
+      <c r="B390" s="1"/>
     </row>
     <row r="391" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B391" s="3"/>
+      <c r="B391" s="1"/>
     </row>
     <row r="392" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B392" s="3"/>
+      <c r="B392" s="1"/>
     </row>
     <row r="393" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B393" s="3"/>
+      <c r="B393" s="1"/>
     </row>
     <row r="394" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B394" s="3"/>
+      <c r="B394" s="1"/>
     </row>
     <row r="395" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B395" s="3"/>
+      <c r="B395" s="1"/>
     </row>
     <row r="396" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B396" s="3"/>
+      <c r="B396" s="1"/>
     </row>
     <row r="397" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B397" s="3"/>
+      <c r="B397" s="1"/>
     </row>
     <row r="398" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B398" s="3"/>
+      <c r="B398" s="1"/>
     </row>
     <row r="399" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B399" s="3"/>
+      <c r="B399" s="1"/>
     </row>
     <row r="400" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B400" s="3"/>
+      <c r="B400" s="1"/>
     </row>
     <row r="401" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B401" s="3"/>
+      <c r="B401" s="1"/>
     </row>
     <row r="402" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B402" s="3"/>
+      <c r="B402" s="1"/>
     </row>
     <row r="403" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B403" s="3"/>
+      <c r="B403" s="1"/>
     </row>
     <row r="404" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B404" s="3"/>
+      <c r="B404" s="1"/>
     </row>
     <row r="405" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B405" s="3"/>
+      <c r="B405" s="1"/>
     </row>
     <row r="406" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B406" s="3"/>
+      <c r="B406" s="1"/>
     </row>
     <row r="407" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B407" s="3"/>
+      <c r="B407" s="1"/>
     </row>
     <row r="408" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B408" s="3"/>
+      <c r="B408" s="1"/>
     </row>
     <row r="409" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B409" s="3"/>
+      <c r="B409" s="1"/>
     </row>
     <row r="410" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B410" s="3"/>
+      <c r="B410" s="1"/>
     </row>
     <row r="411" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B411" s="3"/>
+      <c r="B411" s="1"/>
     </row>
     <row r="412" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B412" s="3"/>
+      <c r="B412" s="1"/>
     </row>
     <row r="413" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B413" s="3"/>
+      <c r="B413" s="1"/>
     </row>
     <row r="414" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B414" s="3"/>
+      <c r="B414" s="1"/>
     </row>
     <row r="415" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B415" s="3"/>
+      <c r="B415" s="1"/>
     </row>
     <row r="416" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B416" s="3"/>
+      <c r="B416" s="1"/>
     </row>
     <row r="417" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B417" s="3"/>
+      <c r="B417" s="1"/>
     </row>
     <row r="418" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B418" s="3"/>
+      <c r="B418" s="1"/>
     </row>
     <row r="419" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B419" s="3"/>
+      <c r="B419" s="1"/>
     </row>
     <row r="420" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B420" s="3"/>
+      <c r="B420" s="1"/>
     </row>
     <row r="421" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B421" s="3"/>
+      <c r="B421" s="1"/>
     </row>
     <row r="422" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B422" s="3"/>
+      <c r="B422" s="1"/>
     </row>
     <row r="423" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B423" s="3"/>
+      <c r="B423" s="1"/>
     </row>
     <row r="424" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B424" s="3"/>
+      <c r="B424" s="1"/>
     </row>
     <row r="425" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B425" s="3"/>
+      <c r="B425" s="1"/>
     </row>
     <row r="426" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B426" s="3"/>
+      <c r="B426" s="1"/>
     </row>
     <row r="427" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B427" s="3"/>
+      <c r="B427" s="1"/>
     </row>
     <row r="428" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B428" s="3"/>
+      <c r="B428" s="1"/>
     </row>
     <row r="429" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B429" s="3"/>
+      <c r="B429" s="1"/>
     </row>
     <row r="430" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B430" s="3"/>
+      <c r="B430" s="1"/>
     </row>
     <row r="431" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B431" s="3"/>
+      <c r="B431" s="1"/>
     </row>
     <row r="432" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B432" s="3"/>
+      <c r="B432" s="1"/>
     </row>
     <row r="433" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B433" s="3"/>
+      <c r="B433" s="1"/>
     </row>
     <row r="434" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B434" s="3"/>
+      <c r="B434" s="1"/>
     </row>
     <row r="435" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B435" s="3"/>
+      <c r="B435" s="1"/>
     </row>
     <row r="436" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B436" s="3"/>
+      <c r="B436" s="1"/>
     </row>
     <row r="437" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B437" s="3"/>
+      <c r="B437" s="1"/>
     </row>
     <row r="438" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B438" s="3"/>
+      <c r="B438" s="1"/>
     </row>
     <row r="439" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B439" s="3"/>
+      <c r="B439" s="1"/>
     </row>
     <row r="440" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B440" s="3"/>
+      <c r="B440" s="1"/>
     </row>
     <row r="441" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B441" s="3"/>
+      <c r="B441" s="1"/>
     </row>
     <row r="442" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B442" s="3"/>
+      <c r="B442" s="1"/>
     </row>
     <row r="443" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B443" s="3"/>
+      <c r="B443" s="1"/>
     </row>
     <row r="444" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B444" s="3"/>
+      <c r="B444" s="1"/>
     </row>
     <row r="445" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B445" s="3"/>
+      <c r="B445" s="1"/>
     </row>
     <row r="446" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B446" s="3"/>
+      <c r="B446" s="1"/>
     </row>
     <row r="447" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B447" s="3"/>
+      <c r="B447" s="1"/>
     </row>
     <row r="448" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B448" s="3"/>
+      <c r="B448" s="1"/>
     </row>
     <row r="449" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B449" s="3"/>
+      <c r="B449" s="1"/>
     </row>
     <row r="450" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B450" s="3"/>
+      <c r="B450" s="1"/>
     </row>
     <row r="451" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B451" s="3"/>
+      <c r="B451" s="1"/>
     </row>
     <row r="452" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B452" s="3"/>
+      <c r="B452" s="1"/>
     </row>
     <row r="453" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B453" s="3"/>
+      <c r="B453" s="1"/>
     </row>
     <row r="454" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B454" s="3"/>
+      <c r="B454" s="1"/>
     </row>
     <row r="455" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B455" s="3"/>
+      <c r="B455" s="1"/>
     </row>
     <row r="456" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B456" s="3"/>
+      <c r="B456" s="1"/>
     </row>
     <row r="457" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B457" s="3"/>
+      <c r="B457" s="1"/>
     </row>
     <row r="458" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B458" s="3"/>
+      <c r="B458" s="1"/>
     </row>
     <row r="459" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B459" s="3"/>
+      <c r="B459" s="1"/>
     </row>
     <row r="460" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B460" s="3"/>
+      <c r="B460" s="1"/>
     </row>
     <row r="461" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B461" s="3"/>
+      <c r="B461" s="1"/>
     </row>
     <row r="462" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B462" s="3"/>
+      <c r="B462" s="1"/>
     </row>
     <row r="463" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B463" s="3"/>
+      <c r="B463" s="1"/>
     </row>
     <row r="464" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B464" s="3"/>
+      <c r="B464" s="1"/>
     </row>
     <row r="465" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B465" s="3"/>
+      <c r="B465" s="1"/>
     </row>
     <row r="466" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B466" s="3"/>
+      <c r="B466" s="1"/>
     </row>
     <row r="467" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B467" s="3"/>
+      <c r="B467" s="1"/>
     </row>
     <row r="468" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B468" s="3"/>
+      <c r="B468" s="1"/>
     </row>
     <row r="469" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B469" s="3"/>
+      <c r="B469" s="1"/>
     </row>
     <row r="470" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B470" s="3"/>
-    </row>
-    <row r="471" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B471" s="3"/>
-    </row>
-    <row r="472" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B472" s="3"/>
-    </row>
-    <row r="473" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B473" s="3"/>
-    </row>
-    <row r="474" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B474" s="3"/>
-    </row>
-    <row r="475" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B475" s="3"/>
-    </row>
-    <row r="476" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B476" s="3"/>
-    </row>
-    <row r="477" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B477" s="3"/>
-    </row>
-    <row r="478" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B478" s="3"/>
-    </row>
-    <row r="479" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B479" s="3"/>
-    </row>
-    <row r="480" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B480" s="3"/>
-    </row>
-    <row r="481" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B481" s="3"/>
-    </row>
-    <row r="482" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B482" s="3"/>
+      <c r="B470" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1" display="https://dev-suny-geneseo.pantheonsite.io/academic-program-finder/accounting" xr:uid="{C3770CB4-E37A-2841-8D1F-5ED298614624}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
need to fix the menu
</commit_message>
<xml_diff>
--- a/basic_page.xlsx
+++ b/basic_page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/purva/Desktop/SUNY Geneseo Playwright/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C8A91B-FCA0-7B47-AD12-3F1E73C0F338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7CC9FE-4306-DB48-AB05-A7A42AB25911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="459">
   <si>
     <t>urso</t>
   </si>
@@ -1377,14 +1377,50 @@
     <t>basic</t>
   </si>
   <si>
-    <t>/biology</t>
+    <t>/steinhauer/</t>
+  </si>
+  <si>
+    <t>menu not found on wordpress</t>
+  </si>
+  <si>
+    <t>/aac/</t>
+  </si>
+  <si>
+    <t>/accounting/</t>
+  </si>
+  <si>
+    <t>/rotc/</t>
+  </si>
+  <si>
+    <t>/academic-program-finder/biochemistry/</t>
+  </si>
+  <si>
+    <t>/cit/</t>
+  </si>
+  <si>
+    <t>Menu matched</t>
+  </si>
+  <si>
+    <t>Menu not found on drupal and wp content is similar</t>
+  </si>
+  <si>
+    <t>Menu items missing on wordpress</t>
+  </si>
+  <si>
+    <t>"HOME" menu item missing from menu</t>
+  </si>
+  <si>
+    <t>Appears "Selected menu is empty or could not be loaded"</t>
+  </si>
+  <si>
+    <t>career-design/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1420,6 +1456,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1458,7 +1499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1469,6 +1510,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1775,19 +1821,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B286"/>
+  <dimension ref="A1:D286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47.5" customWidth="1"/>
-    <col min="2" max="2" width="45.1640625" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>443</v>
       </c>
@@ -1795,60 +1842,96 @@
         <v>444</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>445</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="96" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="96" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="112" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-    </row>
-    <row r="8" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="1"/>
     </row>

</xml_diff>